<commit_message>
All - Delete Lambda project and edit RMOB
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9005" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9055" uniqueCount="170">
   <si>
     <t>Script Num</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>2024-04-22</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>2024-04-25</t>
   </si>
 </sst>
 </file>
@@ -961,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
RMOB - Edit the regression file
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\RMOB_Offical_Testing\src\main\java\P04_Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159D8FAC-51CB-40DB-843C-5EB12C1C2DF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B34C6F5-E22C-4CCF-AF3B-90F759D3DC09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
   <si>
     <t>Script Num</t>
   </si>
@@ -75,37 +75,28 @@
     <t>SKIP SCRIPTS =</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Login</t>
+    <t/>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Load or Pay credit card</t>
   </si>
   <si>
     <t>EN</t>
   </si>
   <si>
-    <t>2024-04-28</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Check account details</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Edit POS limit</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Deactive or active contactless</t>
-  </si>
-  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>2024-04-29</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Check net worth statment chasrts</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -270,11 +261,12 @@
       <font>
         <b/>
         <i val="0"/>
+        <strike val="0"/>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -294,12 +286,11 @@
       <font>
         <b/>
         <i val="0"/>
-        <strike val="0"/>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -582,26 +573,26 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="9.140625" style="1" collapsed="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="74.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="22.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="28.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.6640625" collapsed="true"/>
+    <col min="9" max="11" style="1" width="9.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="7.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="18.44140625" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>7</v>
@@ -621,7 +612,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -631,7 +622,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,41 +643,17 @@
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>24</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="E4" s="8"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>24</v>
-      </c>
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="I5" s="11" t="s">
@@ -699,22 +666,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>25</v>
-      </c>
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="I6" s="11"/>
@@ -723,22 +680,12 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>24</v>
-      </c>
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="I7" s="11"/>
@@ -747,7 +694,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -761,7 +708,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -777,10 +724,10 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12">
         <f>COUNTIF(E1:E100, "*PASS*")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -794,12 +741,22 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="I11" s="12"/>
@@ -808,7 +765,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -822,7 +779,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -838,10 +795,10 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13">
         <f>COUNTIF(E1:E100, "*FAIL*")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -855,7 +812,7 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
@@ -869,12 +826,22 @@
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="I16" s="13"/>
@@ -883,7 +850,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
@@ -902,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="6"/>
@@ -916,7 +883,7 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="6"/>
@@ -930,7 +897,7 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="6"/>
@@ -944,7 +911,7 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="6"/>
@@ -953,7 +920,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="6"/>
@@ -962,7 +929,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="6"/>
@@ -971,7 +938,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="6"/>
@@ -980,7 +947,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="6"/>
@@ -989,7 +956,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="6"/>
@@ -998,7 +965,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="6"/>
@@ -1007,7 +974,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="6"/>
@@ -1016,7 +983,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -1025,7 +992,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
@@ -1034,7 +1001,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
@@ -1043,7 +1010,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
@@ -1052,7 +1019,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
@@ -1061,7 +1028,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
@@ -1070,7 +1037,7 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
@@ -1079,7 +1046,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
@@ -1088,7 +1055,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
@@ -1097,7 +1064,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
@@ -1106,7 +1073,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
@@ -1115,7 +1082,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
@@ -1124,7 +1091,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
@@ -1133,7 +1100,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
@@ -1142,7 +1109,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
@@ -1151,7 +1118,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
@@ -1160,7 +1127,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
@@ -1169,7 +1136,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
@@ -1178,7 +1145,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
@@ -1187,7 +1154,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
@@ -1196,7 +1163,7 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
@@ -1205,7 +1172,7 @@
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
@@ -1214,7 +1181,7 @@
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
@@ -1223,7 +1190,7 @@
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
@@ -1232,7 +1199,7 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="6"/>
@@ -1241,14 +1208,14 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -1319,14 +1286,14 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E100">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E4)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",E4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E4)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1342,7 +1309,7 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
RMOB - Add new sctips and edit readme.md
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\RMOB_Offical_Testing\src\main\java\P04_Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A217564-039D-4646-9CDF-6ABAFCC2758D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B286BB2-37DA-49E4-9C83-A7BAA95F5D11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="58">
   <si>
     <t>Script Num</t>
   </si>
@@ -141,37 +141,70 @@
     <t>Money express transfer</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Charity donation transfer</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Zakaty transfe</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Link my account</t>
+  </si>
+  <si>
+    <t>2024-05-06</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Unlink my account</t>
+  </si>
+  <si>
+    <t>2024-05-08</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Apply for pre-paid</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Apply for a salary card</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Charity donation transfer</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Zakaty transfe</t>
-  </si>
-  <si>
-    <t>2024-05-05</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Link my account</t>
-  </si>
-  <si>
-    <t>2024-05-06</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Unlink my account</t>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Apply for a multi currency card</t>
+  </si>
+  <si>
+    <t>2024-05-21</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply for personal loan </t>
+  </si>
+  <si>
+    <t>2024-05-22</t>
   </si>
 </sst>
 </file>
@@ -303,9 +336,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,6 +346,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -645,7 +678,7 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -723,7 +756,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -731,8 +764,8 @@
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
@@ -740,15 +773,15 @@
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="I5" s="11" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="I5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10">
         <v>50</v>
       </c>
     </row>
@@ -758,13 +791,13 @@
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5"/>
@@ -772,13 +805,13 @@
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5"/>
@@ -786,13 +819,13 @@
       <c r="C8" s="6"/>
       <c r="D8" s="5"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
@@ -800,17 +833,17 @@
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="I9" s="12" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="I9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12">
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11">
         <f>COUNTIF(E1:E100, "*PASS*")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -819,13 +852,13 @@
       <c r="C10" s="6"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
@@ -833,13 +866,13 @@
       <c r="C11" s="6"/>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
@@ -847,13 +880,13 @@
       <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
@@ -861,17 +894,17 @@
       <c r="C13" s="6"/>
       <c r="D13" s="5"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="I13" s="13" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="I13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13">
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12">
         <f>COUNTIF(E1:E100, "*FAIL*")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -880,13 +913,13 @@
       <c r="C14" s="6"/>
       <c r="D14" s="5"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
@@ -894,13 +927,13 @@
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7"/>
@@ -908,13 +941,13 @@
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
@@ -932,17 +965,17 @@
       <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="I17" s="9" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="I17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9">
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13">
         <f>COUNTIF(E1:E100, "*SKIP*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -961,13 +994,13 @@
       <c r="E18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
@@ -985,13 +1018,13 @@
       <c r="E19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
@@ -1009,13 +1042,13 @@
       <c r="E20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
@@ -1033,8 +1066,8 @@
       <c r="E21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
@@ -1052,8 +1085,8 @@
       <c r="E22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
@@ -1071,15 +1104,15 @@
       <c r="E23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>26</v>
@@ -1090,15 +1123,15 @@
       <c r="E24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>26</v>
@@ -1109,8 +1142,8 @@
       <c r="E25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
@@ -1118,8 +1151,8 @@
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
@@ -1127,18 +1160,18 @@
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>16</v>
@@ -1146,18 +1179,18 @@
       <c r="E28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>16</v>
@@ -1165,8 +1198,8 @@
       <c r="E29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="5"/>
@@ -1174,8 +1207,8 @@
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
@@ -1183,8 +1216,8 @@
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="5"/>
@@ -1192,8 +1225,8 @@
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="5"/>
@@ -1201,17 +1234,27 @@
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="A34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="5"/>
@@ -1219,8 +1262,8 @@
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="5"/>
@@ -1228,26 +1271,46 @@
       <c r="C36" s="6"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+      <c r="A37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
+      <c r="A38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="5"/>
@@ -1255,8 +1318,8 @@
       <c r="C39" s="6"/>
       <c r="D39" s="5"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="5"/>
@@ -1264,8 +1327,8 @@
       <c r="C40" s="6"/>
       <c r="D40" s="5"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="5"/>
@@ -1273,8 +1336,8 @@
       <c r="C41" s="6"/>
       <c r="D41" s="5"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="5"/>
@@ -1282,8 +1345,8 @@
       <c r="C42" s="6"/>
       <c r="D42" s="5"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="5"/>
@@ -1291,8 +1354,8 @@
       <c r="C43" s="6"/>
       <c r="D43" s="5"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
@@ -1300,8 +1363,8 @@
       <c r="C44" s="6"/>
       <c r="D44" s="5"/>
       <c r="E44" s="8"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="5"/>
@@ -1309,8 +1372,8 @@
       <c r="C45" s="6"/>
       <c r="D45" s="5"/>
       <c r="E45" s="8"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="5"/>
@@ -1318,8 +1381,8 @@
       <c r="C46" s="6"/>
       <c r="D46" s="5"/>
       <c r="E46" s="8"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="5"/>
@@ -1327,8 +1390,8 @@
       <c r="C47" s="6"/>
       <c r="D47" s="5"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="5"/>
@@ -1336,8 +1399,8 @@
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="5"/>
@@ -1345,8 +1408,8 @@
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="5"/>
@@ -1354,8 +1417,8 @@
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
@@ -1363,17 +1426,27 @@
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
+      <c r="A52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" s="5"/>
@@ -1381,8 +1454,8 @@
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54"/>
@@ -1400,6 +1473,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="M5:M8"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="F53:G53"/>
@@ -1416,50 +1533,6 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E100">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SKIP">

</xml_diff>

<commit_message>
RMOB - Remove all warnings
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="59">
   <si>
     <t>Script Num</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>2024-05-22</t>
+  </si>
+  <si>
+    <t>2024-05-23</t>
   </si>
 </sst>
 </file>
@@ -756,7 +759,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
RMOB - Add Refinance
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\RMOB_Offical_Testing\src\main\java\P04_Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B286BB2-37DA-49E4-9C83-A7BAA95F5D11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA8882D-DEB9-44A1-8D7C-94335C6CCBD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="660" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>Script Num</t>
   </si>
@@ -186,18 +186,12 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
     <t>Apply for a multi currency card</t>
   </si>
   <si>
-    <t>2024-05-21</t>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
@@ -208,6 +202,15 @@
   </si>
   <si>
     <t>2024-05-23</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Refinance</t>
+  </si>
+  <si>
+    <t>2024-05-26</t>
   </si>
 </sst>
 </file>
@@ -339,6 +342,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,9 +355,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -680,24 +683,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="74.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="22.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="28.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.6640625" collapsed="true"/>
-    <col min="9" max="11" style="1" width="9.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="7.6640625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="18.44140625" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="15.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="74.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="11" width="9.109375" style="1" collapsed="1"/>
+    <col min="12" max="12" width="7.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.44140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
@@ -759,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -767,8 +770,8 @@
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
@@ -776,15 +779,15 @@
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="I5" s="10" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="I5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10">
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11">
         <v>50</v>
       </c>
     </row>
@@ -794,13 +797,13 @@
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5"/>
@@ -808,13 +811,13 @@
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5"/>
@@ -822,13 +825,13 @@
       <c r="C8" s="6"/>
       <c r="D8" s="5"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
@@ -836,17 +839,17 @@
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="11" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="I9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11">
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12">
         <f>COUNTIF(E1:E100, "*PASS*")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -855,13 +858,13 @@
       <c r="C10" s="6"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
@@ -869,13 +872,13 @@
       <c r="C11" s="6"/>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
@@ -883,13 +886,13 @@
       <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
@@ -897,15 +900,15 @@
       <c r="C13" s="6"/>
       <c r="D13" s="5"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="I13" s="12" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="I13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13">
         <f>COUNTIF(E1:E100, "*FAIL*")</f>
         <v>5</v>
       </c>
@@ -916,13 +919,13 @@
       <c r="C14" s="6"/>
       <c r="D14" s="5"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
@@ -930,13 +933,13 @@
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7"/>
@@ -944,13 +947,13 @@
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
@@ -968,15 +971,15 @@
       <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="I17" s="13" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="I17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9">
         <f>COUNTIF(E1:E100, "*SKIP*")</f>
         <v>1</v>
       </c>
@@ -997,13 +1000,13 @@
       <c r="E18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
@@ -1021,13 +1024,13 @@
       <c r="E19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
@@ -1045,13 +1048,13 @@
       <c r="E20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
@@ -1069,8 +1072,8 @@
       <c r="E21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
@@ -1088,8 +1091,8 @@
       <c r="E22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
@@ -1107,8 +1110,8 @@
       <c r="E23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
@@ -1126,8 +1129,8 @@
       <c r="E24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
@@ -1145,8 +1148,8 @@
       <c r="E25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
@@ -1154,8 +1157,8 @@
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
@@ -1163,8 +1166,8 @@
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="7" t="s">
@@ -1182,8 +1185,8 @@
       <c r="E28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
@@ -1201,8 +1204,8 @@
       <c r="E29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="5"/>
@@ -1210,8 +1213,8 @@
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
@@ -1219,8 +1222,8 @@
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="5"/>
@@ -1228,8 +1231,8 @@
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="5"/>
@@ -1237,8 +1240,8 @@
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
@@ -1256,8 +1259,8 @@
       <c r="E34" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="5"/>
@@ -1265,8 +1268,8 @@
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="5"/>
@@ -1274,15 +1277,15 @@
       <c r="C36" s="6"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>45</v>
@@ -1293,8 +1296,8 @@
       <c r="E37" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
@@ -1312,8 +1315,8 @@
       <c r="E38" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="5"/>
@@ -1321,8 +1324,8 @@
       <c r="C39" s="6"/>
       <c r="D39" s="5"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="5"/>
@@ -1330,8 +1333,8 @@
       <c r="C40" s="6"/>
       <c r="D40" s="5"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="5"/>
@@ -1339,8 +1342,8 @@
       <c r="C41" s="6"/>
       <c r="D41" s="5"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="5"/>
@@ -1348,8 +1351,8 @@
       <c r="C42" s="6"/>
       <c r="D42" s="5"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="5"/>
@@ -1357,8 +1360,8 @@
       <c r="C43" s="6"/>
       <c r="D43" s="5"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
@@ -1366,8 +1369,8 @@
       <c r="C44" s="6"/>
       <c r="D44" s="5"/>
       <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="5"/>
@@ -1375,8 +1378,8 @@
       <c r="C45" s="6"/>
       <c r="D45" s="5"/>
       <c r="E45" s="8"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="5"/>
@@ -1384,8 +1387,8 @@
       <c r="C46" s="6"/>
       <c r="D46" s="5"/>
       <c r="E46" s="8"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="5"/>
@@ -1393,8 +1396,8 @@
       <c r="C47" s="6"/>
       <c r="D47" s="5"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="5"/>
@@ -1402,8 +1405,8 @@
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="5"/>
@@ -1411,8 +1414,8 @@
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="5"/>
@@ -1420,8 +1423,8 @@
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
@@ -1429,18 +1432,18 @@
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>16</v>
@@ -1448,17 +1451,27 @@
       <c r="E52" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
+      <c r="A53" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54"/>
@@ -1476,50 +1489,6 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="F53:G53"/>
@@ -1536,6 +1505,50 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="M5:M8"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E100">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SKIP">

</xml_diff>

<commit_message>
RMOB - Modify project
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\RMOB_Offical_Testing\src\main\java\P04_Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF31D9F1-28C3-496E-80FB-8801D146428B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFD6446-18AF-49FC-A571-D643D4EB30B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Script Num</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t xml:space="preserve">Script Name </t>
   </si>
@@ -72,22 +69,31 @@
     <t>SKIP SCRIPTS =</t>
   </si>
   <si>
-    <t>4.14.0 - M2 - V2.uat</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Login</t>
+    <t>4.15.0 - M0 - V2.uat</t>
+  </si>
+  <si>
+    <t>25/09/2024</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Money express transfer</t>
   </si>
   <si>
     <t>EN</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>2024-08-20</t>
+    <t xml:space="preserve"> FAIL </t>
+  </si>
+  <si>
+    <t>2024-10-03</t>
   </si>
 </sst>
 </file>
@@ -219,6 +225,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -229,9 +238,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -874,47 +880,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:G10"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="74.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="9.109375" style="1" collapsed="1"/>
-    <col min="12" max="12" width="7.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.109375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="74.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="28.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="9" max="11" style="1" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="14">
-        <v>45441</v>
+        <v>4</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -924,594 +930,594 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F3" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="I5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="I5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="5"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="I9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="I9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12">
         <f>COUNTIF(E1:E100, "*PASS*")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="5"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="I13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="I13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13">
         <f>COUNTIF(E1:E100, "*FAIL*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="5"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-    </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-    </row>
-    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="I17" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="I17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9">
         <f>COUNTIF(E1:E100, "*SKIP*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
       <c r="D39" s="5"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
       <c r="D40" s="5"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
       <c r="D41" s="5"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
       <c r="D42" s="5"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
       <c r="D43" s="5"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
       <c r="D44" s="5"/>
       <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
       <c r="D45" s="5"/>
       <c r="E45" s="8"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
       <c r="D46" s="5"/>
       <c r="E46" s="8"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
       <c r="D47" s="5"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="6"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54" s="8"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -1520,50 +1526,6 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="F53:G53"/>
@@ -1580,8 +1542,52 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="M5:M8"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
-  <conditionalFormatting sqref="E33 E36 E4:E31 E43:E100">
+  <conditionalFormatting sqref="E33 E36 E43:E100 E4:E31">
     <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",E4)))</formula>
     </cfRule>
@@ -1678,11 +1684,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1CCC0-0B11-4751-9C6C-B478225C7EB5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
One2 - Setup Project
</commit_message>
<xml_diff>
--- a/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
+++ b/RMOB_Offical_Testing/src/main/java/P04_Utils/Report_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\RMOB_Offical_Testing\src\main\java\P04_Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DCA207-AECF-4841-A7CC-DA3451A1AF99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07B21C9-0D9D-4EA7-8596-967A3ED6C57A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="49">
   <si>
     <t xml:space="preserve">Script Name </t>
   </si>
@@ -78,82 +78,82 @@
     <t>Test Data</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>35</t>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>2024-10-30</t>
+  </si>
+  <si>
+    <t>Edit POS limit</t>
+  </si>
+  <si>
+    <t>Load or Pay credit card</t>
+  </si>
+  <si>
+    <t>Transfer from credit card</t>
+  </si>
+  <si>
+    <t>Between my account transfer</t>
+  </si>
+  <si>
+    <t>Within riyad bank trnasfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FAIL </t>
+  </si>
+  <si>
+    <t>Local transfer</t>
+  </si>
+  <si>
+    <t>International transfer</t>
+  </si>
+  <si>
+    <t>WU transfer</t>
+  </si>
+  <si>
+    <t>Money express transfer</t>
+  </si>
+  <si>
+    <t>Charity donation transfer</t>
+  </si>
+  <si>
+    <t>Zakaty transfer</t>
+  </si>
+  <si>
+    <t>request to pay transfer</t>
+  </si>
+  <si>
+    <t>Apply for a credit card</t>
+  </si>
+  <si>
+    <t>Apply for a pre-paid</t>
+  </si>
+  <si>
+    <t>Apply for a multi currency card</t>
+  </si>
+  <si>
+    <t>Add riyad bank beneficiary</t>
+  </si>
+  <si>
+    <t>Add local beneficiary</t>
+  </si>
+  <si>
+    <t>Add international beneficiary</t>
+  </si>
+  <si>
+    <t>Add money express beneficiary</t>
+  </si>
+  <si>
+    <t>Add a bill</t>
+  </si>
+  <si>
+    <t>Pay a bill</t>
   </si>
   <si>
     <t>36</t>
@@ -162,22 +162,22 @@
     <t>37</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>38</t>
   </si>
   <si>
-    <t>Add international beneficiary</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FAIL </t>
-  </si>
-  <si>
-    <t>2024-10-07</t>
+    <t>39</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +228,12 @@
       <b/>
       <sz val="26"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,8 +315,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,6 +330,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -334,44 +343,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <b/>
@@ -962,29 +934,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M12"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="74.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="28.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="9" max="11" style="1" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="74.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="22.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="28.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" style="1" width="16.6640625" collapsed="true"/>
+    <col min="9" max="11" style="1" width="9.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="7.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="18.44140625" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -999,12 +970,12 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1014,7 +985,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1030,30 +1001,46 @@
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4" s="8"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="I5" s="11" t="s">
@@ -1063,17 +1050,25 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="I6" s="11"/>
@@ -1082,14 +1077,22 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="I7" s="11"/>
@@ -1098,14 +1101,22 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
+    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="I8" s="11"/>
@@ -1114,14 +1125,22 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="I9" s="12" t="s">
@@ -1131,18 +1150,26 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12">
-        <f>COUNTIF(E1:E100, "*PASS*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
+        <f>COUNTIF(E1:E74, "*PASS*")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="I10" s="12"/>
@@ -1151,14 +1178,22 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="I11" s="12"/>
@@ -1167,14 +1202,22 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="I12" s="12"/>
@@ -1183,14 +1226,22 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
+    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="I13" s="13" t="s">
@@ -1200,18 +1251,26 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13">
-        <f>COUNTIF(E1:E100, "*FAIL*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
+        <f>COUNTIF(E1:E74, "*FAIL*")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="I14" s="13"/>
@@ -1220,14 +1279,22 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
+    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="I15" s="13"/>
@@ -1236,14 +1303,22 @@
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="I16" s="13"/>
@@ -1252,422 +1327,487 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9">
-        <f>COUNTIF(E1:E100, "*SKIP*")</f>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14">
+        <f>COUNTIF(E1:E74, "*SKIP*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7">
-        <v>15</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A21" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A24" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="9">
+        <v>99333996</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="7"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
       <c r="E28" s="8"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="8"/>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8"/>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="8"/>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="8"/>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="8"/>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="8"/>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>47</v>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="8"/>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="8"/>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="8"/>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="8"/>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="8"/>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="8"/>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="8"/>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="8"/>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="8"/>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
+      </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="8"/>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>24</v>
+      </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="8"/>
+    <row r="53" spans="6:7" x14ac:dyDescent="0.4">
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="E58"/>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="M5:M8"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="F53:G53"/>
@@ -1684,137 +1824,72 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
   </mergeCells>
-  <conditionalFormatting sqref="E33 E36 E43:E100 E4:E31">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="SKIP">
+  <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="E24:E74 E4:E16">
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="SKIP">
       <formula>NOT(ISERROR(SEARCH("SKIP",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="19" priority="30" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="28" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E32)))</formula>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E32)))</formula>
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E32)))</formula>
+    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E34)))</formula>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",E19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E34)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E34)))</formula>
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E35)))</formula>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E35)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E35)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E37)))</formula>
+  <conditionalFormatting sqref="E21:E23">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",E21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E37)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E37)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E38)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40:E42">
+  <conditionalFormatting sqref="E18">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",E40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SKIP",E18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",E18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PASS",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1830,7 +1905,7 @@
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>